<commit_message>
updates to data files and scripts
</commit_message>
<xml_diff>
--- a/data/bam_names_to_metadata.xlsx
+++ b/data/bam_names_to_metadata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomsasani/harrislab/bxd_mutator_ms/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625B55AC-FFC9-EB48-A738-461DD16961FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8F9BA2-4196-CF4D-8D70-A7BA4BD4DCAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{BB955B75-A553-FA40-B469-2318236E5DDA}"/>
+    <workbookView xWindow="36300" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{BB955B75-A553-FA40-B469-2318236E5DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="663">
   <si>
     <t>Expanded name</t>
   </si>
@@ -2014,6 +2036,15 @@
   </si>
   <si>
     <t>4512-JFI-0362_BXD155_phased_possorted_bam</t>
+  </si>
+  <si>
+    <t>backcrossed?</t>
+  </si>
+  <si>
+    <t>backcross_string</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -2417,10 +2448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EB6DD8-BC66-A743-BCB5-9E528FB0F248}">
-  <dimension ref="A1:L244"/>
+  <dimension ref="A1:N244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="I108" workbookViewId="0">
+      <selection activeCell="K128" sqref="K128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2438,7 +2469,7 @@
     <col min="11" max="11" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>505</v>
       </c>
@@ -2475,8 +2506,14 @@
       <c r="L1" s="6" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M1" s="6" t="s">
+        <v>660</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>506</v>
       </c>
@@ -2513,8 +2550,15 @@
       <c r="L2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="b">
+        <f>ISNUMBER(SEARCH(N2, K2))</f>
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>507</v>
       </c>
@@ -2551,8 +2595,15 @@
       <c r="L3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="b">
+        <f t="shared" ref="M3:M66" si="0">ISNUMBER(SEARCH(N3, K3))</f>
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>508</v>
       </c>
@@ -2589,8 +2640,15 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>509</v>
       </c>
@@ -2627,8 +2685,15 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>510</v>
       </c>
@@ -2665,8 +2730,15 @@
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>511</v>
       </c>
@@ -2703,8 +2775,15 @@
       <c r="L7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>512</v>
       </c>
@@ -2741,8 +2820,15 @@
       <c r="L8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>513</v>
       </c>
@@ -2779,8 +2865,15 @@
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>514</v>
       </c>
@@ -2817,8 +2910,15 @@
       <c r="L10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>515</v>
       </c>
@@ -2855,8 +2955,15 @@
       <c r="L11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>516</v>
       </c>
@@ -2893,8 +3000,15 @@
       <c r="L12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>517</v>
       </c>
@@ -2931,8 +3045,15 @@
       <c r="L13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>518</v>
       </c>
@@ -2969,8 +3090,15 @@
       <c r="L14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>519</v>
       </c>
@@ -3007,8 +3135,15 @@
       <c r="L15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>520</v>
       </c>
@@ -3045,8 +3180,15 @@
       <c r="L16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>521</v>
       </c>
@@ -3083,8 +3225,15 @@
       <c r="L17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>522</v>
       </c>
@@ -3121,8 +3270,15 @@
       <c r="L18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M18" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>523</v>
       </c>
@@ -3159,8 +3315,15 @@
       <c r="L19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M19" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>524</v>
       </c>
@@ -3197,8 +3360,15 @@
       <c r="L20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N20" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>525</v>
       </c>
@@ -3235,8 +3405,15 @@
       <c r="L21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M21" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N21" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>526</v>
       </c>
@@ -3273,8 +3450,15 @@
       <c r="L22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M22" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N22" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>527</v>
       </c>
@@ -3311,8 +3495,15 @@
       <c r="L23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M23" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N23" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>528</v>
       </c>
@@ -3349,8 +3540,15 @@
       <c r="L24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M24" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N24" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>529</v>
       </c>
@@ -3387,8 +3585,15 @@
       <c r="L25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M25" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>530</v>
       </c>
@@ -3425,8 +3630,15 @@
       <c r="L26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M26" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N26" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>531</v>
       </c>
@@ -3463,8 +3675,15 @@
       <c r="L27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M27" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>532</v>
       </c>
@@ -3501,8 +3720,15 @@
       <c r="L28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M28" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>533</v>
       </c>
@@ -3539,8 +3765,15 @@
       <c r="L29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M29" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>534</v>
       </c>
@@ -3577,8 +3810,15 @@
       <c r="L30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M30" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>535</v>
       </c>
@@ -3615,8 +3855,15 @@
       <c r="L31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N31" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>536</v>
       </c>
@@ -3653,8 +3900,15 @@
       <c r="L32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M32" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N32" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>537</v>
       </c>
@@ -3691,8 +3945,15 @@
       <c r="L33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M33" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N33" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>538</v>
       </c>
@@ -3729,8 +3990,15 @@
       <c r="L34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M34" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N34" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>539</v>
       </c>
@@ -3767,8 +4035,15 @@
       <c r="L35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M35" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N35" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>540</v>
       </c>
@@ -3805,8 +4080,15 @@
       <c r="L36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M36" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N36" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>541</v>
       </c>
@@ -3843,8 +4125,15 @@
       <c r="L37">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M37" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N37" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>542</v>
       </c>
@@ -3881,8 +4170,15 @@
       <c r="L38">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M38" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N38" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>543</v>
       </c>
@@ -3919,8 +4215,15 @@
       <c r="L39">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M39" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>544</v>
       </c>
@@ -3957,8 +4260,15 @@
       <c r="L40">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M40" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N40" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>545</v>
       </c>
@@ -3995,8 +4305,15 @@
       <c r="L41">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N41" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>546</v>
       </c>
@@ -4033,8 +4350,15 @@
       <c r="L42">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N42" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>547</v>
       </c>
@@ -4071,8 +4395,15 @@
       <c r="L43">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N43" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>548</v>
       </c>
@@ -4109,8 +4440,15 @@
       <c r="L44">
         <v>14</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M44" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N44" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>549</v>
       </c>
@@ -4147,8 +4485,15 @@
       <c r="L45">
         <v>9</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N45" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>550</v>
       </c>
@@ -4185,8 +4530,15 @@
       <c r="L46">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N46" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>551</v>
       </c>
@@ -4223,8 +4575,15 @@
       <c r="L47">
         <v>9</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N47" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>552</v>
       </c>
@@ -4261,8 +4620,15 @@
       <c r="L48">
         <v>9</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M48" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N48" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>553</v>
       </c>
@@ -4299,8 +4665,15 @@
       <c r="L49">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M49" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N49" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>554</v>
       </c>
@@ -4337,8 +4710,15 @@
       <c r="L50">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M50" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N50" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>555</v>
       </c>
@@ -4375,8 +4755,15 @@
       <c r="L51">
         <v>9</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M51" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N51" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>556</v>
       </c>
@@ -4407,8 +4794,15 @@
       <c r="L52">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M52" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N52" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>557</v>
       </c>
@@ -4445,8 +4839,15 @@
       <c r="L53">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M53" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N53" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>558</v>
       </c>
@@ -4483,8 +4884,15 @@
       <c r="L54">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M54" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N54" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>559</v>
       </c>
@@ -4521,8 +4929,15 @@
       <c r="L55">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M55" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N55" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>560</v>
       </c>
@@ -4559,8 +4974,15 @@
       <c r="L56">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M56" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N56" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>561</v>
       </c>
@@ -4597,8 +5019,15 @@
       <c r="L57">
         <v>10</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M57" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N57" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>562</v>
       </c>
@@ -4635,8 +5064,15 @@
       <c r="L58">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M58" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N58" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>563</v>
       </c>
@@ -4673,8 +5109,15 @@
       <c r="L59">
         <v>10</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M59" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N59" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>564</v>
       </c>
@@ -4711,8 +5154,15 @@
       <c r="L60">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M60" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N60" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>565</v>
       </c>
@@ -4749,8 +5199,15 @@
       <c r="L61">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M61" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N61" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>566</v>
       </c>
@@ -4787,8 +5244,15 @@
       <c r="L62">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M62" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N62" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>567</v>
       </c>
@@ -4825,8 +5289,15 @@
       <c r="L63">
         <v>10</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M63" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N63" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>568</v>
       </c>
@@ -4863,8 +5334,15 @@
       <c r="L64">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M64" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N64" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>569</v>
       </c>
@@ -4901,8 +5379,15 @@
       <c r="L65">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M65" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N65" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>570</v>
       </c>
@@ -4939,8 +5424,15 @@
       <c r="L66">
         <v>10</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M66" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N66" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>571</v>
       </c>
@@ -4977,8 +5469,15 @@
       <c r="L67">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M67" t="b">
+        <f t="shared" ref="M67:M130" si="1">ISNUMBER(SEARCH(N67, K67))</f>
+        <v>0</v>
+      </c>
+      <c r="N67" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>572</v>
       </c>
@@ -5015,8 +5514,15 @@
       <c r="L68">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M68" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N68" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>573</v>
       </c>
@@ -5053,8 +5559,15 @@
       <c r="L69">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M69" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N69" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>574</v>
       </c>
@@ -5091,8 +5604,15 @@
       <c r="L70">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M70" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N70" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>575</v>
       </c>
@@ -5129,8 +5649,15 @@
       <c r="L71">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M71" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N71" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>658</v>
       </c>
@@ -5167,8 +5694,15 @@
       <c r="L72">
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M72" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N72" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>576</v>
       </c>
@@ -5205,8 +5739,15 @@
       <c r="L73">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M73" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N73" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>577</v>
       </c>
@@ -5237,8 +5778,15 @@
       <c r="L74">
         <v>10</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M74" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N74" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>578</v>
       </c>
@@ -5275,8 +5823,15 @@
       <c r="L75">
         <v>10</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M75" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N75" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>579</v>
       </c>
@@ -5313,8 +5868,15 @@
       <c r="L76">
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M76" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N76" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>580</v>
       </c>
@@ -5351,8 +5913,15 @@
       <c r="L77">
         <v>10</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M77" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N77" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>581</v>
       </c>
@@ -5389,8 +5958,15 @@
       <c r="L78">
         <v>10</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M78" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N78" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>582</v>
       </c>
@@ -5427,8 +6003,15 @@
       <c r="L79">
         <v>10</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M79" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N79" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>583</v>
       </c>
@@ -5465,8 +6048,15 @@
       <c r="L80">
         <v>10</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M80" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N80" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>584</v>
       </c>
@@ -5503,8 +6093,15 @@
       <c r="L81">
         <v>10</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M81" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N81" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>585</v>
       </c>
@@ -5541,8 +6138,15 @@
       <c r="L82">
         <v>10</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M82" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N82" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>586</v>
       </c>
@@ -5579,8 +6183,15 @@
       <c r="L83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M83" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N83" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>587</v>
       </c>
@@ -5617,8 +6228,15 @@
       <c r="L84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M84" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N84" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>588</v>
       </c>
@@ -5655,8 +6273,15 @@
       <c r="L85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M85" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N85" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>589</v>
       </c>
@@ -5693,8 +6318,15 @@
       <c r="L86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M86" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N86" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>590</v>
       </c>
@@ -5731,8 +6363,15 @@
       <c r="L87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M87" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N87" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>591</v>
       </c>
@@ -5769,8 +6408,15 @@
       <c r="L88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M88" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N88" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>592</v>
       </c>
@@ -5807,8 +6453,15 @@
       <c r="L89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M89" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N89" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>593</v>
       </c>
@@ -5845,8 +6498,15 @@
       <c r="L90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M90" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N90" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>594</v>
       </c>
@@ -5883,8 +6543,15 @@
       <c r="L91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M91" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N91" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>595</v>
       </c>
@@ -5921,8 +6588,15 @@
       <c r="L92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M92" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N92" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>596</v>
       </c>
@@ -5959,8 +6633,15 @@
       <c r="L93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M93" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N93" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>597</v>
       </c>
@@ -5997,8 +6678,15 @@
       <c r="L94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M94" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N94" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>598</v>
       </c>
@@ -6035,8 +6723,15 @@
       <c r="L95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M95" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N95" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>599</v>
       </c>
@@ -6073,8 +6768,15 @@
       <c r="L96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M96" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N96" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>600</v>
       </c>
@@ -6111,8 +6813,15 @@
       <c r="L97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M97" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N97" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>601</v>
       </c>
@@ -6149,8 +6858,15 @@
       <c r="L98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M98" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N98" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>602</v>
       </c>
@@ -6187,8 +6903,15 @@
       <c r="L99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M99" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N99" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>603</v>
       </c>
@@ -6225,8 +6948,15 @@
       <c r="L100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M100" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N100" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>657</v>
       </c>
@@ -6263,8 +6993,15 @@
       <c r="L101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M101" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N101" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>604</v>
       </c>
@@ -6301,8 +7038,15 @@
       <c r="L102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M102" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N102" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>659</v>
       </c>
@@ -6339,8 +7083,15 @@
       <c r="L103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M103" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N103" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>605</v>
       </c>
@@ -6377,8 +7128,15 @@
       <c r="L104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M104" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N104" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>606</v>
       </c>
@@ -6415,8 +7173,15 @@
       <c r="L105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M105" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N105" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>607</v>
       </c>
@@ -6453,8 +7218,15 @@
       <c r="L106">
         <v>8</v>
       </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M106" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N106" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>608</v>
       </c>
@@ -6491,8 +7263,15 @@
       <c r="L107">
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M107" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N107" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>609</v>
       </c>
@@ -6529,8 +7308,15 @@
       <c r="L108">
         <v>9</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M108" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N108" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>610</v>
       </c>
@@ -6567,8 +7353,15 @@
       <c r="L109">
         <v>9</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M109" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N109" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>611</v>
       </c>
@@ -6605,8 +7398,15 @@
       <c r="L110">
         <v>9</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M110" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N110" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>612</v>
       </c>
@@ -6643,8 +7443,15 @@
       <c r="L111">
         <v>9</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M111" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N111" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>613</v>
       </c>
@@ -6681,8 +7488,15 @@
       <c r="L112">
         <v>9</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M112" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N112" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>614</v>
       </c>
@@ -6719,8 +7533,15 @@
       <c r="L113">
         <v>9</v>
       </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M113" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N113" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>615</v>
       </c>
@@ -6757,8 +7578,15 @@
       <c r="L114">
         <v>9</v>
       </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M114" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N114" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>616</v>
       </c>
@@ -6795,8 +7623,15 @@
       <c r="L115">
         <v>9</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M115" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N115" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>617</v>
       </c>
@@ -6833,8 +7668,15 @@
       <c r="L116">
         <v>9</v>
       </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M116" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N116" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>618</v>
       </c>
@@ -6871,8 +7713,15 @@
       <c r="L117">
         <v>9</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M117" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N117" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>619</v>
       </c>
@@ -6909,8 +7758,15 @@
       <c r="L118">
         <v>9</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M118" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N118" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>620</v>
       </c>
@@ -6947,8 +7803,15 @@
       <c r="L119">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M119" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N119" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>621</v>
       </c>
@@ -6985,8 +7848,15 @@
       <c r="L120">
         <v>9</v>
       </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M120" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N120" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>622</v>
       </c>
@@ -7023,8 +7893,15 @@
       <c r="L121">
         <v>9</v>
       </c>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M121" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N121" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>623</v>
       </c>
@@ -7061,8 +7938,15 @@
       <c r="L122">
         <v>9</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M122" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N122" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>624</v>
       </c>
@@ -7099,8 +7983,15 @@
       <c r="L123">
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M123" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N123" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>625</v>
       </c>
@@ -7137,8 +8028,15 @@
       <c r="L124">
         <v>9</v>
       </c>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M124" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N124" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>626</v>
       </c>
@@ -7175,8 +8073,15 @@
       <c r="L125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M125" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N125" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>627</v>
       </c>
@@ -7213,8 +8118,15 @@
       <c r="L126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M126" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N126" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>628</v>
       </c>
@@ -7251,8 +8163,15 @@
       <c r="L127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M127" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N127" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>656</v>
       </c>
@@ -7289,8 +8208,15 @@
       <c r="L128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M128" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N128" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>629</v>
       </c>
@@ -7327,8 +8253,15 @@
       <c r="L129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M129" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N129" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>630</v>
       </c>
@@ -7365,8 +8298,15 @@
       <c r="L130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M130" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N130" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>631</v>
       </c>
@@ -7403,8 +8343,15 @@
       <c r="L131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M131" t="b">
+        <f t="shared" ref="M131:M154" si="2">ISNUMBER(SEARCH(N131, K131))</f>
+        <v>0</v>
+      </c>
+      <c r="N131" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>632</v>
       </c>
@@ -7441,8 +8388,15 @@
       <c r="L132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M132" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N132" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>633</v>
       </c>
@@ -7479,8 +8433,15 @@
       <c r="L133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M133" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N133" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>634</v>
       </c>
@@ -7517,8 +8478,15 @@
       <c r="L134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M134" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N134" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>635</v>
       </c>
@@ -7555,8 +8523,15 @@
       <c r="L135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M135" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N135" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>636</v>
       </c>
@@ -7593,8 +8568,15 @@
       <c r="L136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M136" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N136" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>637</v>
       </c>
@@ -7631,8 +8613,15 @@
       <c r="L137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M137" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N137" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>638</v>
       </c>
@@ -7669,8 +8658,15 @@
       <c r="L138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M138" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N138" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>639</v>
       </c>
@@ -7707,8 +8703,15 @@
       <c r="L139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M139" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N139" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>640</v>
       </c>
@@ -7745,8 +8748,15 @@
       <c r="L140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M140" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N140" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>641</v>
       </c>
@@ -7783,8 +8793,15 @@
       <c r="L141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M141" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N141" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>642</v>
       </c>
@@ -7821,8 +8838,15 @@
       <c r="L142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M142" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N142" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>643</v>
       </c>
@@ -7859,8 +8883,15 @@
       <c r="L143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M143" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N143" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>644</v>
       </c>
@@ -7897,8 +8928,15 @@
       <c r="L144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M144" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N144" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>645</v>
       </c>
@@ -7935,8 +8973,15 @@
       <c r="L145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M145" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N145" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>646</v>
       </c>
@@ -7973,8 +9018,15 @@
       <c r="L146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M146" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N146" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>647</v>
       </c>
@@ -8011,8 +9063,15 @@
       <c r="L147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M147" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N147" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>648</v>
       </c>
@@ -8046,8 +9105,15 @@
       <c r="L148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M148" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N148" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>649</v>
       </c>
@@ -8081,8 +9147,15 @@
       <c r="L149">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M149" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N149" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>650</v>
       </c>
@@ -8116,8 +9189,15 @@
       <c r="L150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M150" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N150" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>651</v>
       </c>
@@ -8151,8 +9231,15 @@
       <c r="L151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M151" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N151" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>652</v>
       </c>
@@ -8186,8 +9273,15 @@
       <c r="L152">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M152" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="N152" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>653</v>
       </c>
@@ -8221,8 +9315,15 @@
       <c r="L153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M153" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N153" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>654</v>
       </c>
@@ -8256,8 +9357,21 @@
       <c r="L154">
         <v>0</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M154" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N154" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M157" cm="1">
+        <f t="array" ref="M157">SUM(--(M2:M154))</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="J160" s="4"/>
       <c r="K160" s="4"/>
     </row>

</xml_diff>